<commit_message>
arrangement d'une ligne dans le JE pour quelle rentre dans la bd
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01_JE_04_SysExp.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01_JE_04_SysExp.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -285,9 +285,6 @@
     <t>PSVitaOS</t>
   </si>
   <si>
-    <t>PlayStation Vita operating system</t>
-  </si>
-  <si>
     <t>Version 3</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>Système d'exploitation MAC</t>
+  </si>
+  <si>
+    <t>PSVita OS</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,7 +439,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -651,7 +651,7 @@
   <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2007,7 +2007,7 @@
         <v>9</v>
       </c>
       <c r="F79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2041,7 +2041,7 @@
         <v>8</v>
       </c>
       <c r="F81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2052,13 +2052,13 @@
         <v>88</v>
       </c>
       <c r="C82" t="s">
+        <v>96</v>
+      </c>
+      <c r="D82" t="s">
         <v>89</v>
       </c>
-      <c r="D82" t="s">
+      <c r="F82" t="s">
         <v>90</v>
-      </c>
-      <c r="F82" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2066,16 +2066,16 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>91</v>
+      </c>
+      <c r="C83" t="s">
         <v>92</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>93</v>
       </c>
-      <c r="D83" t="s">
-        <v>94</v>
-      </c>
       <c r="F83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>